<commit_message>
Removed SMA for GPIO header placement.
</commit_message>
<xml_diff>
--- a/01_Docs/nRF52840_QFN48_Pin_Mapping.xlsx
+++ b/01_Docs/nRF52840_QFN48_Pin_Mapping.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Kicad\NRF_LoRa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Kicad\NRF_LoRa\01_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936450D7-68CF-4A55-AD68-D7BD51AA4A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760E0ACA-A799-474C-B2CB-57C99047187D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
   <si>
     <t>Pin #</t>
   </si>
@@ -61,18 +61,12 @@
     <t>P0.05</t>
   </si>
   <si>
-    <t>P0.07</t>
-  </si>
-  <si>
     <t>P0.08</t>
   </si>
   <si>
     <t>P1.08</t>
   </si>
   <si>
-    <t>P1.09</t>
-  </si>
-  <si>
     <t>P0.23</t>
   </si>
   <si>
@@ -106,24 +100,12 @@
     <t>Status LED</t>
   </si>
   <si>
-    <t>Button Input</t>
-  </si>
-  <si>
-    <t>UART CTS (opt)</t>
-  </si>
-  <si>
-    <t>UART RTS (opt)</t>
-  </si>
-  <si>
     <t>UART RX</t>
   </si>
   <si>
     <t>UART TX</t>
   </si>
   <si>
-    <t>FuelGauge ALERT (opt)</t>
-  </si>
-  <si>
     <t>I²C SDA</t>
   </si>
   <si>
@@ -151,24 +133,12 @@
     <t>LED_STATUS</t>
   </si>
   <si>
-    <t>BTN_USER</t>
-  </si>
-  <si>
-    <t>FTDI_CTS</t>
-  </si>
-  <si>
-    <t>FTDI_RTS</t>
-  </si>
-  <si>
     <t>MCU_RX</t>
   </si>
   <si>
     <t>MCU_TX</t>
   </si>
   <si>
-    <t>FUEL_ALERT</t>
-  </si>
-  <si>
     <t>I2C_SDA</t>
   </si>
   <si>
@@ -196,24 +166,12 @@
     <t>Optional GPIO LED</t>
   </si>
   <si>
-    <t>Pull-up required</t>
-  </si>
-  <si>
-    <t>Optional if using CTS</t>
-  </si>
-  <si>
-    <t>Optional if using RTS</t>
-  </si>
-  <si>
     <t>From FTDI TX</t>
   </si>
   <si>
     <t>To FTDI RX</t>
   </si>
   <si>
-    <t>MAX17048 ALERT</t>
-  </si>
-  <si>
     <t>To OLED/sensors</t>
   </si>
   <si>
@@ -226,34 +184,16 @@
     <t>Debug interface</t>
   </si>
   <si>
-    <t>P0.28</t>
-  </si>
-  <si>
-    <t>P0.29</t>
-  </si>
-  <si>
-    <t>P0.30</t>
-  </si>
-  <si>
     <t>GPIO1</t>
   </si>
   <si>
     <t>GPIO2</t>
   </si>
   <si>
-    <t>GPIO3</t>
-  </si>
-  <si>
-    <t>P0.31</t>
-  </si>
-  <si>
-    <t>GPIO4</t>
-  </si>
-  <si>
     <t>NotUsed</t>
   </si>
   <si>
-    <t>2,3,29,30,40,39,4,19,20,23,38</t>
+    <t>2,3,6,29,30,40,39,4,19,20,23,38,41,42,43,44</t>
   </si>
 </sst>
 </file>
@@ -621,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -659,13 +599,13 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -676,13 +616,13 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -693,13 +633,13 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -710,13 +650,13 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -727,13 +667,13 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -744,13 +684,13 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -761,13 +701,13 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>58</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -778,220 +718,142 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="E12" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E13" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="E15" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
         <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="E16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>26</v>
-      </c>
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>27</v>
-      </c>
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>41</v>
-      </c>
-      <c r="B19" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>42</v>
-      </c>
-      <c r="B20" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>43</v>
-      </c>
-      <c r="B21" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>44</v>
-      </c>
-      <c r="B22" t="s">
-        <v>74</v>
-      </c>
-      <c r="C22" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>77</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>